<commit_message>
Updated dates in survey data files
</commit_message>
<xml_diff>
--- a/messy_project_directory/EXCEL_Spreadsheets/Survey_Data_Tidy.xlsx
+++ b/messy_project_directory/EXCEL_Spreadsheets/Survey_Data_Tidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Fiber/Desktop/Git/tfcb-homework01/messy_project_directory/EXCEL_Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48284177-7760-764B-A635-91AB9C13E965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0CC794-2618-A64F-8393-D17ECE032F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="1460" windowWidth="27400" windowHeight="15580" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="1780" windowWidth="27400" windowHeight="15580" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -102,22 +102,22 @@
     <t>Scale Calibration (Y)es/(N)o</t>
   </si>
   <si>
-    <t>????-3-11</t>
-  </si>
-  <si>
-    <t>????-4-8</t>
-  </si>
-  <si>
-    <t>????-5-6</t>
-  </si>
-  <si>
-    <t>????-5-18</t>
-  </si>
-  <si>
-    <t>????-6-9</t>
-  </si>
-  <si>
-    <t>????-7-8</t>
+    <t>????-03-11</t>
+  </si>
+  <si>
+    <t>????-04-08</t>
+  </si>
+  <si>
+    <t>????-05-06</t>
+  </si>
+  <si>
+    <t>????-05-18</t>
+  </si>
+  <si>
+    <t>????-07-08</t>
+  </si>
+  <si>
+    <t>????-06-09</t>
   </si>
 </sst>
 </file>
@@ -125,7 +125,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -172,7 +172,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,7 +572,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -616,7 +616,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -641,8 +641,8 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1728,7 +1728,7 @@
         <v>2014</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>6</v>
@@ -1754,7 +1754,7 @@
         <v>2014</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
@@ -1780,7 +1780,7 @@
         <v>2014</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>

</xml_diff>